<commit_message>
Optimize US9412_01 and HPFS_01
</commit_message>
<xml_diff>
--- a/data/NGQ_HPFS_01_data.xlsx
+++ b/data/NGQ_HPFS_01_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="7680" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -228,7 +228,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -263,7 +263,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +631,7 @@
         <v>31</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="W2" t="s">
         <v>34</v>

</xml_diff>